<commit_message>
update report to include more figures
</commit_message>
<xml_diff>
--- a/results/model_performance.xlsx
+++ b/results/model_performance.xlsx
@@ -423,10 +423,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.6290410521696344</v>
+        <v>0.6505652753855917</v>
       </c>
       <c r="C2">
-        <v>0.3164498027395917</v>
+        <v>0.3239546012577356</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -434,10 +434,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.4855371476668514</v>
+        <v>0.5104454560234108</v>
       </c>
       <c r="C3">
-        <v>0.6948988377098579</v>
+        <v>0.6908527463133148</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -445,10 +445,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.8929623197160764</v>
+        <v>0.8967191460497662</v>
       </c>
       <c r="C4">
-        <v>0.20487356030079</v>
+        <v>0.2115856651939126</v>
       </c>
     </row>
   </sheetData>
@@ -477,7 +477,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0.5282451990198115</v>
+        <v>0.5388968606257292</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -485,7 +485,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.5190765994862335</v>
+        <v>0.539271932520575</v>
       </c>
     </row>
   </sheetData>
@@ -517,10 +517,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.6933236063594285</v>
+        <v>0.7155667407823686</v>
       </c>
       <c r="C2">
-        <v>0.3320366007342063</v>
+        <v>0.3400419524916378</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -528,10 +528,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.5658064913469237</v>
+        <v>0.5951471305478784</v>
       </c>
       <c r="C3">
-        <v>0.6521739130434783</v>
+        <v>0.6409489207095533</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -539,10 +539,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.8950410807651089</v>
+        <v>0.8970777430619371</v>
       </c>
       <c r="C4">
-        <v>0.2227122381477398</v>
+        <v>0.2314043209876543</v>
       </c>
     </row>
   </sheetData>
@@ -571,7 +571,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0.6335975910773362</v>
+        <v>0.6400000894026562</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -579,7 +579,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.5796424322879851</v>
+        <v>0.6024655943721613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>